<commit_message>
Cleared up the clutter
</commit_message>
<xml_diff>
--- a/data/voltage_050225_10.xlsx
+++ b/data/voltage_050225_10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpuente2\Documents\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93612106-3028-4257-90D9-6967CC49EB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB04C4E-CB5A-49FA-BBC4-649C9359B791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18700" xr2:uid="{F914C2BB-B448-462A-B265-911E1C6F56BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Relative Time</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>DeflY 7 V</t>
+  </si>
+  <si>
+    <t>Range 16-0 V</t>
+  </si>
+  <si>
+    <t>Step 0.05 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of sweeps </t>
+  </si>
+  <si>
+    <t>Number of measuements per step</t>
   </si>
 </sst>
 </file>
@@ -449,15 +461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E6C66F-6452-4D1C-A7D7-C289DB0F6607}">
-  <dimension ref="A1:C6421"/>
+  <dimension ref="A1:D6421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="28.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -478,8 +493,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.6707909999999999E-2</v>
       </c>
@@ -489,8 +507,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>18.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3.3411181999999998E-2</v>
       </c>
@@ -500,8 +521,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5.0118060999999998E-2</v>
       </c>
@@ -511,8 +535,11 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6.6824969999999997E-2</v>
       </c>
@@ -522,8 +549,11 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>11.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.10224999999999999</v>
       </c>
@@ -533,8 +563,11 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.118956728</v>
       </c>
@@ -544,8 +577,11 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.13566</v>
       </c>
@@ -555,8 +591,11 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.152364</v>
       </c>
@@ -566,8 +605,11 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.16907160700000001</v>
       </c>
@@ -577,8 +619,11 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.49999939399999999</v>
       </c>
@@ -588,37 +633,64 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.51670506100000002</v>
       </c>
       <c r="B13">
         <v>-955.12925084439996</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.533409091</v>
       </c>
       <c r="B14">
         <v>-955.12841272449998</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.55011451600000005</v>
       </c>
       <c r="B15">
         <v>-955.12400878569997</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.56682069700000004</v>
       </c>
       <c r="B16">
         <v>-955.12838224749999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>